<commit_message>
Comments added and employeehistory table modified
</commit_message>
<xml_diff>
--- a/assets/empAuditData.xlsx
+++ b/assets/empAuditData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>EmpId</t>
   </si>
@@ -26,31 +26,37 @@
     <t>Salary</t>
   </si>
   <si>
+    <t>45227</t>
+  </si>
+  <si>
+    <t>Aswin raam P</t>
+  </si>
+  <si>
+    <t>Jan 08 2019</t>
+  </si>
+  <si>
+    <t>Feb 28 2019</t>
+  </si>
+  <si>
+    <t>Mar 28 2019</t>
+  </si>
+  <si>
+    <t>Apr 30 2019</t>
+  </si>
+  <si>
     <t>45228</t>
   </si>
   <si>
     <t>Pradeep kumar G</t>
   </si>
   <si>
-    <t>45227</t>
-  </si>
-  <si>
-    <t>Aswin raam P</t>
-  </si>
-  <si>
     <t>45229</t>
   </si>
   <si>
-    <t>Praveen Kumar S</t>
-  </si>
-  <si>
     <t>Praveen kumar S</t>
   </si>
   <si>
     <t>45209</t>
-  </si>
-  <si>
-    <t>Sonali Bharti</t>
   </si>
   <si>
     <t>Sonali bharti</t>
@@ -98,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -125,8 +131,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
-        <v>43473.0</v>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>15000.0</v>
@@ -139,11 +145,11 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>43496.0</v>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>11613.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="4">
@@ -153,11 +159,11 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>43524.0</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>5858.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="5">
@@ -167,78 +173,78 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="n">
-        <v>43552.0</v>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>15000.0</v>
+        <v>20800.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>43585.0</v>
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>20800.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="n">
-        <v>43473.0</v>
-      </c>
       <c r="D7" t="n">
-        <v>15000.0</v>
+        <v>5858.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>43496.0</v>
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>11613.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="n">
-        <v>43524.0</v>
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
       </c>
       <c r="D9" t="n">
-        <v>15000.0</v>
+        <v>20800.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="n">
-        <v>43552.0</v>
       </c>
       <c r="D10" t="n">
         <v>15000.0</v>
@@ -246,27 +252,27 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="n">
-        <v>43585.0</v>
-      </c>
       <c r="D11" t="n">
-        <v>20800.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="n">
-        <v>43473.0</v>
       </c>
       <c r="D12" t="n">
         <v>15000.0</v>
@@ -274,27 +280,27 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="n">
-        <v>43524.0</v>
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v>15000.0</v>
+        <v>20800.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="n">
-        <v>43552.0</v>
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
       </c>
       <c r="D14" t="n">
         <v>15000.0</v>
@@ -302,27 +308,27 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="n">
-        <v>43585.0</v>
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>20800.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="n">
-        <v>43473.0</v>
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
       </c>
       <c r="D16" t="n">
         <v>15000.0</v>
@@ -330,57 +336,15 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="n">
-        <v>43496.0</v>
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
       </c>
       <c r="D17" t="n">
-        <v>11613.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="n">
-        <v>43524.0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>15000.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="n">
-        <v>43552.0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>15000.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="n">
-        <v>43585.0</v>
-      </c>
-      <c r="D20" t="n">
         <v>20800.0</v>
       </c>
     </row>

</xml_diff>